<commit_message>
Homework 4 Final Commit
- Final updates for homework 4.
- Includes last submission into canvas.
</commit_message>
<xml_diff>
--- a/hw4/Statistics.xlsx
+++ b/hw4/Statistics.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12795" xr2:uid="{A0C3BF6E-1765-4091-AB7C-338678C18B64}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12795" activeTab="1" xr2:uid="{A0C3BF6E-1765-4091-AB7C-338678C18B64}"/>
   </bookViews>
   <sheets>
     <sheet name="Problem2" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Problem1" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -25,12 +26,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
   <si>
     <t>Loop Unrolls</t>
   </si>
   <si>
     <t>Execution Time (ns)</t>
+  </si>
+  <si>
+    <t>Block Size</t>
   </si>
 </sst>
 </file>
@@ -87,13 +91,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -584,7 +589,514 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Execution Time</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> vs. Software Loop Block Size</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Final</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$6</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>8619930491</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3207318191.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4412285429.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5708939374.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7254412656.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-ED96-4798-8A20-305C9976B421}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="530893088"/>
+        <c:axId val="530892760"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="530893088"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Software</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Loop Block Size</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="530892760"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="530892760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Execution</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Time (ns)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="530893088"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1140,8 +1652,535 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{830D7E33-73FA-4320-85B0-EC46EF263E0D}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="123" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{67C6A3FF-C5D4-4646-B80C-A44B12215A0B}">
   <sheetPr/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="123" workbookViewId="0" zoomToFit="1"/>
@@ -1162,6 +2201,39 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{01C4488D-EC2D-47A1-82B2-C0E721DDF5A3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8673171" cy="6295793"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D99EDA4-E4E9-46EC-90B9-EF6B0F27F311}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1481,64 +2553,164 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35E6B4E5-1EBE-4E2C-B876-35554A75BA01}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B6"/>
+      <selection activeCell="D1" sqref="D1:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>0</v>
       </c>
       <c r="B2" s="3">
         <v>187712</v>
       </c>
+      <c r="D2" s="2">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3">
+        <v>8619930491</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0</v>
+      </c>
+      <c r="H2" s="3">
+        <v>8619930491</v>
+      </c>
+      <c r="J2" s="2">
+        <v>0</v>
+      </c>
+      <c r="K2" s="3">
+        <v>8619930491</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="3">
         <v>176189</v>
       </c>
+      <c r="D3" s="4">
+        <v>16</v>
+      </c>
+      <c r="E3" s="3">
+        <v>3207318191.5</v>
+      </c>
+      <c r="G3" s="4">
+        <v>16</v>
+      </c>
+      <c r="H3" s="6">
+        <v>3207318191.5</v>
+      </c>
+      <c r="J3" s="4">
+        <v>16</v>
+      </c>
+      <c r="K3" s="3">
+        <v>1100131877.5</v>
+      </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>4</v>
       </c>
       <c r="B4" s="3">
         <v>178131.5</v>
       </c>
+      <c r="D4" s="2">
+        <v>32</v>
+      </c>
+      <c r="E4" s="3">
+        <v>4412285429.5</v>
+      </c>
+      <c r="G4" s="2">
+        <v>32</v>
+      </c>
+      <c r="H4" s="6">
+        <v>4412285429.5</v>
+      </c>
+      <c r="J4" s="2">
+        <v>32</v>
+      </c>
+      <c r="K4" s="3">
+        <v>1687166202.5</v>
+      </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>8</v>
       </c>
       <c r="B5" s="3">
         <v>172611</v>
       </c>
+      <c r="D5" s="2">
+        <v>64</v>
+      </c>
+      <c r="E5" s="3">
+        <v>5708939374.5</v>
+      </c>
+      <c r="G5" s="2">
+        <v>64</v>
+      </c>
+      <c r="H5" s="6">
+        <v>5708939374.5</v>
+      </c>
+      <c r="J5" s="2">
+        <v>64</v>
+      </c>
+      <c r="K5" s="3">
+        <v>1676359533.5</v>
+      </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>16</v>
       </c>
       <c r="B6" s="5">
         <v>171303</v>
+      </c>
+      <c r="D6" s="2">
+        <v>128</v>
+      </c>
+      <c r="E6" s="3">
+        <v>7254412656.5</v>
+      </c>
+      <c r="G6" s="2">
+        <v>128</v>
+      </c>
+      <c r="H6" s="6">
+        <v>7254412656.5</v>
+      </c>
+      <c r="J6" s="2">
+        <v>128</v>
+      </c>
+      <c r="K6" s="3">
+        <v>7254412656.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>